<commit_message>
a Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/doc/独立系统接口.xlsx
+++ b/doc/独立系统接口.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="123">
   <si>
     <t>模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,6 +180,377 @@
   </si>
   <si>
     <t>http://xxx/abmember!getMultipleMemberForAccounts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!getMemberCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询用户总数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!checkAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号，密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"account":account, "password":password}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!updateUserTokenForId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"userId":userId,"token":token}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id,新token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abprivilege!getRoleIdForId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"userId":userId}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取用户的权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>授权</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abauth!validAppIdAndSecret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"appId":appid,"secret":secret}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>appId,secret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"accounts":accounts}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据成员账号获取成员id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">获取初始权限 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>http://xxx/abprivilege!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>getInitLoginPriv</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 短信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!getMemberIdsByAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!getTextCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"phone":phone}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!saveTextCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"phone":phone,"code":code}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机、验证码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存短信验证码记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取短信验证码记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!valideOldPwd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证旧密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!updateUserPwdForPhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"phone":phone,"newPwd":newPwd}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号，新密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>依据手机号更新密码</t>
+  </si>
+  <si>
+    <t>http://xxx/abmember!updateUserPwdForAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"account":account,"oldPwd":oldPwd}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"account":account,"newPwd":newPwd}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号，新密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>依据账号更新密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!saveSelectedPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!saveTempPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!isUsedPic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!getUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"userId":userId,"picName":picName}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"userId":userId,"logName":logName}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!delUserLogos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"userId":userId}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成员id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成员id,成员头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成员id，成员头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成员头像，选择好的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存成员头像，上传</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除成员头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认是否正在使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">获取成员头像 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!getMemberIdForAccount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"account":account}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据账号获取id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!getMultipleMemberForIds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"ids":ids}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据多id获取成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abranch!getBranchMemberByMemberIds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"ids":ids}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取部门成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abmember!getMemberForId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"userId":userId}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据id获取单个成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abprivilege!getPrivByUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"groupManager":[]}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取权限根据url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abprivilege!getRolePrivsByPrivs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"privIds":[]}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限id数组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abprivilege!getRolesForIds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"ids":ids}"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -316,13 +687,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -636,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -672,7 +1043,7 @@
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -732,7 +1103,7 @@
     </row>
     <row r="6" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -747,7 +1118,7 @@
     </row>
     <row r="7" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -761,8 +1132,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -775,234 +1146,576 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="3"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="3"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8"/>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="8"/>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="8"/>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8"/>
+      <c r="B12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
+      <c r="B13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
+      <c r="B14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="8"/>
+      <c r="B15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="8"/>
+      <c r="B16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="8"/>
+      <c r="B17" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="9"/>
+      <c r="B18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9"/>
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="8"/>
+      <c r="B22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8"/>
+      <c r="B23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8"/>
+      <c r="B24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="9"/>
+      <c r="B25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="8"/>
+      <c r="B27" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="8"/>
+      <c r="B28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="3"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="1"/>
+    <row r="29" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="8"/>
+      <c r="B29" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="3"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+    <row r="30" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="9"/>
+      <c r="B30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="4"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="4"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="4"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="3"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="3"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A44" s="3"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="3"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A49" s="3"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A50" s="3"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A51" s="3"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A52" s="3"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A53" s="3"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A54" s="3"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A55" s="3"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A56" s="3"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A8"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
+    <hyperlink ref="B11" r:id="rId5"/>
+    <hyperlink ref="B30" r:id="rId6"/>
+    <hyperlink ref="B31" r:id="rId7"/>
+    <hyperlink ref="B18" r:id="rId8"/>
+    <hyperlink ref="B26" r:id="rId9"/>
+    <hyperlink ref="B19" r:id="rId10"/>
+    <hyperlink ref="B20" r:id="rId11"/>
+    <hyperlink ref="B12" r:id="rId12"/>
+    <hyperlink ref="B13" r:id="rId13"/>
+    <hyperlink ref="B14" r:id="rId14"/>
+    <hyperlink ref="B21" r:id="rId15"/>
+    <hyperlink ref="B22" r:id="rId16"/>
+    <hyperlink ref="B23" r:id="rId17"/>
+    <hyperlink ref="B24" r:id="rId18"/>
+    <hyperlink ref="B25" r:id="rId19"/>
+    <hyperlink ref="B15" r:id="rId20"/>
+    <hyperlink ref="B16" r:id="rId21"/>
+    <hyperlink ref="B32" r:id="rId22"/>
+    <hyperlink ref="B17" r:id="rId23"/>
+    <hyperlink ref="B27" r:id="rId24"/>
+    <hyperlink ref="B28" r:id="rId25"/>
+    <hyperlink ref="B29" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <legacyDrawing r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
组织结构接口 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/doc/独立系统接口.xlsx
+++ b/doc/独立系统接口.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="143">
   <si>
     <t>模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -590,15 +590,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"{"id":[],"param":[,]}"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>成员id数组，要取的参数数组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>取指定成员参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"id":[],"param":["id",]}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abranch!getPosition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取职位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/abranch!getBranchTreeAndMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取部门及成员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://xxx/getBranchTree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取部门树</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1057,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1365,13 +1397,13 @@
         <v>131</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1587,7 +1619,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -1604,25 +1636,49 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
@@ -1772,11 +1828,12 @@
       <c r="E59" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A35:A38"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1809,9 +1866,12 @@
     <hyperlink ref="B18" r:id="rId27"/>
     <hyperlink ref="B19" r:id="rId28"/>
     <hyperlink ref="B20" r:id="rId29"/>
+    <hyperlink ref="B36" r:id="rId30"/>
+    <hyperlink ref="B37" r:id="rId31"/>
+    <hyperlink ref="B38" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
-  <legacyDrawing r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
+  <legacyDrawing r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
公司id标识 Signed-off-by: hao_dy <hao_dy@pataw.cn>
</commit_message>
<xml_diff>
--- a/doc/独立系统接口.xlsx
+++ b/doc/独立系统接口.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="153">
   <si>
     <t>模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -663,6 +663,14 @@
   </si>
   <si>
     <t>"{"id":id}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"{"organId":organId}"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -802,6 +810,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -810,9 +821,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1118,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1149,7 +1157,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1166,7 +1174,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1181,7 +1189,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1204,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1211,7 +1219,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1226,7 +1234,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1241,7 +1249,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1256,7 +1264,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1271,7 +1279,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1286,7 +1294,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1301,7 +1309,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1316,7 +1324,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -1331,7 +1339,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>76</v>
       </c>
@@ -1346,7 +1354,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>98</v>
       </c>
@@ -1361,7 +1369,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>102</v>
       </c>
@@ -1376,7 +1384,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>110</v>
       </c>
@@ -1391,7 +1399,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>123</v>
       </c>
@@ -1406,7 +1414,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>127</v>
       </c>
@@ -1421,7 +1429,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>131</v>
       </c>
@@ -1436,8 +1444,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="5" t="s">
         <v>147</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1447,7 +1455,7 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
@@ -1462,7 +1470,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1479,7 +1487,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
         <v>65</v>
       </c>
@@ -1494,7 +1502,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1511,7 +1519,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="1" t="s">
         <v>82</v>
       </c>
@@ -1526,7 +1534,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
         <v>88</v>
       </c>
@@ -1541,7 +1549,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="1" t="s">
         <v>83</v>
       </c>
@@ -1556,7 +1564,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="7"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="1" t="s">
         <v>84</v>
       </c>
@@ -1571,7 +1579,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1588,7 +1596,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="6"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="1" t="s">
         <v>114</v>
       </c>
@@ -1603,7 +1611,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="6"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="1" t="s">
         <v>118</v>
       </c>
@@ -1616,7 +1624,7 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>121</v>
       </c>
@@ -1627,8 +1635,8 @@
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="6"/>
-      <c r="B34" s="8" t="s">
+      <c r="A34" s="7"/>
+      <c r="B34" s="5" t="s">
         <v>149</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1638,7 +1646,7 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="7"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
@@ -1670,7 +1678,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="6" t="s">
         <v>107</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1687,7 +1695,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="6"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="1" t="s">
         <v>135</v>
       </c>
@@ -1702,22 +1710,22 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="6"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="7"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="1" t="s">
         <v>142</v>
       </c>

</xml_diff>